<commit_message>
Atualização: versão estável do SIGMA-Q com base oficial e correções de carregamento
</commit_message>
<xml_diff>
--- a/data/logs/log_classificacoes.xlsx
+++ b/data/logs/log_classificacoes.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C397"/>
+  <dimension ref="A1:C496"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6394,6 +6394,1491 @@
         <v>45968.50253472223</v>
       </c>
     </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>RCA NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C398" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>RUIDO NA HÉLICE</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C399" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>RÁDIO NÃO FUNCIONA/SINTONIZA</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C400" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>GRAVAÇÃO FALHA DE PROCESSO</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C401" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>LUZ DE JIG</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C402" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>FLASH LIGHT FALTANDO COR</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C403" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>MAU CONTATO NA LEITURA DO PEN DRIVE</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C404" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>BATERIA/PILHA NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C405" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>APARELHO COM CORPO ESTRANHO</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C406" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>FALHA DE INJEÇÃO/SERIGRAFIA</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C407" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>SOFTWARE TRAVANDO</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C408" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>PONTO BRILHANTE</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C409" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>TENSÕES VARIANDO</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C410" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>LED/FLASH LIGHT COM LUZ FRACA</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C411" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>DISPLAY NÃO ACENDE</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C412" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>TENSÃO BAIXA</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C413" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>VAZAMENTO DE LUZ</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C414" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>RUÍDO NO ÁUDIO DO MIC/FONE/AUX</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C415" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>CONTROLE COM POUCA SENSIBILIDADE</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C416" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>ABERTURA/GAP</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C417" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>NÃO GRAVA/ATUALIZA</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C418" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>TERRA ABERTO</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C419" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>COATING/SELADOR</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C420" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>ALETA NÃO ABRE/FECHA</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C421" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>EXCESSO DE DÍGITOS</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C422" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>O-CELL COM PELÍCULA</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C423" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>LINHA VERTICAL</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C424" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>POTÊNCIA MÁXIMA</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C425" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>LED NÃO APAGA</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C426" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>INTERFERÊNCIA NA IMAGEM</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C427" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>SEM VÍDEO NO HDMI</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C428" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>LED/DISPLAY PISCANDO</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C429" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>SOFTWARE DESATUALIZADO</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C430" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>VOLUME MÁXIMO NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C431" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>LED COM COR DIFERENTE</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C432" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>PONTO APAGADO</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C433" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>CALÇO/QUADRO APARECENDO</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C434" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>APARELHO NÃO LÊ PEN DRIVE</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C435" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>FALSA FALHA</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C436" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>HI-POT/RIGIDEZ/WI</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C437" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>LED COM LUZ INVERTIDA</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C438" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>EQUIPAMENTO DE TESTE</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C439" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>LINHA HORIZONTAL</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C440" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>RUÍDO NO VENTILADOR</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C441" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>VENTILADOR NÃO GIRA</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C442" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>TECLA DESLOCADA/DANIFICADA</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C443" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>MAL MONTADO</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C444" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>EMPENADO/AMASSADO</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C445" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>TESCON MATERIAL</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C446" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO MIC/FONE/AUX</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C447" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>LIGA/DESLIGA AUTOMATICAMENTE</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C448" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>FALHA VISUAL/MONTAGEM</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C449" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>TESCON FALHA DE PROCESSO</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C450" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>LÂMPADA FRACA/FORTE</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C451" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>CENTELHANDO/RUÍDO</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C452" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>SEM VÍDEO NO RF/ANTENA</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C453" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>LED NÃO ACENDE</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C454" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>FLASH LIGHT NÃO LIGA</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C455" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>APARELHO NÃO DESLIGA</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C456" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>FUNÇÃO INVERTIDA</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C457" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>ÁUDIO OSCILANDO</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C458" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>LÂMPADA NÃO ACENDE</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C459" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>PLACA EM CURTO</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C460" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>CONTROLE NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C461" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>SEM TENSÃO</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C462" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>RISCADO</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C463" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO CANAL DO AF</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C464" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO ALTO-FALANTE</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C465" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>PRATO NÃO GIRA</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C466" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>APARELHO NÃO CARREGA</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C467" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>SEM IMAGEM/SEM BRILHO</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C468" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>MANCHA ESCURA NA TELA</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C469" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>CONTAMINAÇÃO</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C470" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>TECLA DURA</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C471" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>QUEBRADO/DANIFICADO/BATIDO</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C472" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>NÃO COMUNICA</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C473" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>LÂMPADA NÃO APAGA</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C474" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>APARELHO NÃO LIGA</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C475" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>VIBRAÇÃO NO ÁUDIO</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C476" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO CANAL ESQUERDO/FONE</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C477" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>MANCHA</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C478" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>RUÍDO NO ÁUDIO</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C479" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>VOLUME MÍNIMO NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C480" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO CANAL DIREITO/FONE</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C481" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>SEM SINAL DE WI-FI</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C482" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>ESPANADO</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C483" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>TECLAS NÃO ATUAM</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C484" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>VAZAMENTO DE GÁS</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C485" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>VAZAMENTO DE AR</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C486" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>FALTANDO</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C487" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>FORA DO ESPECIFICADO</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C488" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO GERAL</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C489" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO TWEETER</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C490" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>BLUETOOTH NÃO FUNCIONA</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C491" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>NÃO AQUECE</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C492" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>ÁUDIO BAIXO</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C493" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>COM REBARBA</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C494" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>DESLOCADO</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C495" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>FALTANDO DÍGITO NO DISPLAY</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C496" s="2" t="n">
+        <v>45968.50834490741</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove __pycache__ para reconstrução limpa no Streamlit Cloud
</commit_message>
<xml_diff>
--- a/data/logs/log_classificacoes.xlsx
+++ b/data/logs/log_classificacoes.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C496"/>
+  <dimension ref="A1:C793"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7879,6 +7879,4461 @@
         <v>45968.50834490741</v>
       </c>
     </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>RCA NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C497" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>RUIDO NA HÉLICE</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C498" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>RÁDIO NÃO FUNCIONA/SINTONIZA</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C499" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>GRAVAÇÃO FALHA DE PROCESSO</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C500" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>LUZ DE JIG</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C501" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>FLASH LIGHT FALTANDO COR</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C502" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>MAU CONTATO NA LEITURA DO PEN DRIVE</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C503" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>BATERIA/PILHA NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C504" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>APARELHO COM CORPO ESTRANHO</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C505" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>FALHA DE INJEÇÃO/SERIGRAFIA</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C506" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>SOFTWARE TRAVANDO</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C507" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>PONTO BRILHANTE</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C508" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>TENSÕES VARIANDO</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C509" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>LED/FLASH LIGHT COM LUZ FRACA</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C510" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>DISPLAY NÃO ACENDE</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C511" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>TENSÃO BAIXA</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C512" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>VAZAMENTO DE LUZ</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C513" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>RUÍDO NO ÁUDIO DO MIC/FONE/AUX</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C514" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>CONTROLE COM POUCA SENSIBILIDADE</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C515" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>ABERTURA/GAP</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C516" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>NÃO GRAVA/ATUALIZA</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C517" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>TERRA ABERTO</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C518" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>COATING/SELADOR</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C519" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>ALETA NÃO ABRE/FECHA</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C520" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>EXCESSO DE DÍGITOS</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C521" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>O-CELL COM PELÍCULA</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C522" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>LINHA VERTICAL</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C523" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>POTÊNCIA MÁXIMA</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C524" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>LED NÃO APAGA</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C525" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>INTERFERÊNCIA NA IMAGEM</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C526" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>SEM VÍDEO NO HDMI</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C527" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>LED/DISPLAY PISCANDO</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C528" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>SOFTWARE DESATUALIZADO</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C529" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>VOLUME MÁXIMO NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C530" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>LED COM COR DIFERENTE</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C531" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>PONTO APAGADO</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C532" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>CALÇO/QUADRO APARECENDO</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C533" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>APARELHO NÃO LÊ PEN DRIVE</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C534" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>FALSA FALHA</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C535" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>HI-POT/RIGIDEZ/WI</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C536" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>LED COM LUZ INVERTIDA</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C537" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>EQUIPAMENTO DE TESTE</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C538" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>LINHA HORIZONTAL</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C539" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>RUÍDO NO VENTILADOR</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C540" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>VENTILADOR NÃO GIRA</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C541" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>TECLA DESLOCADA/DANIFICADA</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C542" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>MAL MONTADO</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C543" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>EMPENADO/AMASSADO</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C544" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>TESCON MATERIAL</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C545" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO MIC/FONE/AUX</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C546" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>LIGA/DESLIGA AUTOMATICAMENTE</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C547" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>FALHA VISUAL/MONTAGEM</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C548" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>TESCON FALHA DE PROCESSO</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C549" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>LÂMPADA FRACA/FORTE</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C550" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>CENTELHANDO/RUÍDO</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C551" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>SEM VÍDEO NO RF/ANTENA</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C552" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>LED NÃO ACENDE</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C553" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>FLASH LIGHT NÃO LIGA</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C554" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>APARELHO NÃO DESLIGA</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C555" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>FUNÇÃO INVERTIDA</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C556" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>ÁUDIO OSCILANDO</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C557" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>LÂMPADA NÃO ACENDE</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C558" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>PLACA EM CURTO</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C559" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>CONTROLE NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C560" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>SEM TENSÃO</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C561" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>RISCADO</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C562" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO CANAL DO AF</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C563" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO ALTO-FALANTE</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C564" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>PRATO NÃO GIRA</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C565" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>APARELHO NÃO CARREGA</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C566" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>SEM IMAGEM/SEM BRILHO</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C567" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>MANCHA ESCURA NA TELA</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C568" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>CONTAMINAÇÃO</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C569" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>TECLA DURA</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C570" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>QUEBRADO/DANIFICADO/BATIDO</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C571" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>NÃO COMUNICA</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C572" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>LÂMPADA NÃO APAGA</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C573" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>APARELHO NÃO LIGA</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C574" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>VIBRAÇÃO NO ÁUDIO</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C575" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO CANAL ESQUERDO/FONE</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C576" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>MANCHA</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C577" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>RUÍDO NO ÁUDIO</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C578" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>VOLUME MÍNIMO NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C579" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO CANAL DIREITO/FONE</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C580" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>SEM SINAL DE WI-FI</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C581" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>ESPANADO</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C582" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>TECLAS NÃO ATUAM</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C583" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>VAZAMENTO DE GÁS</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C584" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>VAZAMENTO DE AR</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C585" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>FALTANDO</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C586" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>FORA DO ESPECIFICADO</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C587" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO GERAL</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C588" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO TWEETER</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C589" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>BLUETOOTH NÃO FUNCIONA</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C590" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>NÃO AQUECE</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C591" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>ÁUDIO BAIXO</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C592" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>COM REBARBA</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C593" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>DESLOCADO</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C594" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>FALTANDO DÍGITO NO DISPLAY</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C595" s="2" t="n">
+        <v>45968.51327546296</v>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>RCA NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C596" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>RUIDO NA HÉLICE</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C597" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>RÁDIO NÃO FUNCIONA/SINTONIZA</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C598" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>GRAVAÇÃO FALHA DE PROCESSO</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C599" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>LUZ DE JIG</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C600" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>FLASH LIGHT FALTANDO COR</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C601" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>MAU CONTATO NA LEITURA DO PEN DRIVE</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C602" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>BATERIA/PILHA NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C603" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>APARELHO COM CORPO ESTRANHO</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C604" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>FALHA DE INJEÇÃO/SERIGRAFIA</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C605" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>SOFTWARE TRAVANDO</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C606" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>PONTO BRILHANTE</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C607" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>TENSÕES VARIANDO</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C608" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>LED/FLASH LIGHT COM LUZ FRACA</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C609" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>DISPLAY NÃO ACENDE</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C610" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>TENSÃO BAIXA</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C611" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>VAZAMENTO DE LUZ</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C612" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>RUÍDO NO ÁUDIO DO MIC/FONE/AUX</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C613" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>CONTROLE COM POUCA SENSIBILIDADE</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C614" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>ABERTURA/GAP</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C615" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>NÃO GRAVA/ATUALIZA</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C616" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>TERRA ABERTO</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C617" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>COATING/SELADOR</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C618" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>ALETA NÃO ABRE/FECHA</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C619" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>EXCESSO DE DÍGITOS</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C620" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>O-CELL COM PELÍCULA</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C621" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>LINHA VERTICAL</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C622" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>POTÊNCIA MÁXIMA</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C623" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>LED NÃO APAGA</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C624" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>INTERFERÊNCIA NA IMAGEM</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C625" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>SEM VÍDEO NO HDMI</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C626" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>LED/DISPLAY PISCANDO</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C627" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>SOFTWARE DESATUALIZADO</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C628" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>VOLUME MÁXIMO NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C629" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>LED COM COR DIFERENTE</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C630" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>PONTO APAGADO</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C631" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>CALÇO/QUADRO APARECENDO</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C632" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>APARELHO NÃO LÊ PEN DRIVE</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C633" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>FALSA FALHA</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C634" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>HI-POT/RIGIDEZ/WI</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C635" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>LED COM LUZ INVERTIDA</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C636" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>EQUIPAMENTO DE TESTE</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C637" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>LINHA HORIZONTAL</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C638" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>RUÍDO NO VENTILADOR</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C639" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>VENTILADOR NÃO GIRA</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C640" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>TECLA DESLOCADA/DANIFICADA</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C641" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>MAL MONTADO</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C642" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>EMPENADO/AMASSADO</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C643" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>TESCON MATERIAL</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C644" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO MIC/FONE/AUX</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C645" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>LIGA/DESLIGA AUTOMATICAMENTE</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C646" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>FALHA VISUAL/MONTAGEM</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C647" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>TESCON FALHA DE PROCESSO</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C648" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>LÂMPADA FRACA/FORTE</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C649" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>CENTELHANDO/RUÍDO</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C650" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>SEM VÍDEO NO RF/ANTENA</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C651" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>LED NÃO ACENDE</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C652" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>FLASH LIGHT NÃO LIGA</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C653" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>APARELHO NÃO DESLIGA</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C654" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>FUNÇÃO INVERTIDA</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C655" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>ÁUDIO OSCILANDO</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C656" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>LÂMPADA NÃO ACENDE</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C657" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>PLACA EM CURTO</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C658" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>CONTROLE NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C659" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>SEM TENSÃO</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C660" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>RISCADO</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C661" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO CANAL DO AF</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C662" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO ALTO-FALANTE</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C663" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>PRATO NÃO GIRA</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C664" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>APARELHO NÃO CARREGA</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C665" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>SEM IMAGEM/SEM BRILHO</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C666" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>MANCHA ESCURA NA TELA</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C667" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>CONTAMINAÇÃO</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C668" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>TECLA DURA</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C669" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>QUEBRADO/DANIFICADO/BATIDO</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C670" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>NÃO COMUNICA</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C671" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>LÂMPADA NÃO APAGA</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C672" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>APARELHO NÃO LIGA</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C673" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>VIBRAÇÃO NO ÁUDIO</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C674" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO CANAL ESQUERDO/FONE</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C675" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>MANCHA</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C676" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>RUÍDO NO ÁUDIO</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C677" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>VOLUME MÍNIMO NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C678" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO CANAL DIREITO/FONE</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C679" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>SEM SINAL DE WI-FI</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C680" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>ESPANADO</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C681" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>TECLAS NÃO ATUAM</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C682" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>VAZAMENTO DE GÁS</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C683" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>VAZAMENTO DE AR</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C684" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>FALTANDO</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C685" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>FORA DO ESPECIFICADO</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C686" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO GERAL</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C687" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO TWEETER</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C688" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>BLUETOOTH NÃO FUNCIONA</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C689" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>NÃO AQUECE</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C690" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>ÁUDIO BAIXO</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C691" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>COM REBARBA</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C692" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>DESLOCADO</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C693" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>FALTANDO DÍGITO NO DISPLAY</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C694" s="2" t="n">
+        <v>45968.51824074074</v>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>RCA NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C695" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>RUIDO NA HÉLICE</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C696" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>RÁDIO NÃO FUNCIONA/SINTONIZA</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C697" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>GRAVAÇÃO FALHA DE PROCESSO</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C698" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>LUZ DE JIG</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C699" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>FLASH LIGHT FALTANDO COR</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C700" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>MAU CONTATO NA LEITURA DO PEN DRIVE</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C701" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>BATERIA/PILHA NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C702" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>APARELHO COM CORPO ESTRANHO</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C703" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>FALHA DE INJEÇÃO/SERIGRAFIA</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C704" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>SOFTWARE TRAVANDO</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C705" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>PONTO BRILHANTE</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C706" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>TENSÕES VARIANDO</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C707" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>LED/FLASH LIGHT COM LUZ FRACA</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C708" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>DISPLAY NÃO ACENDE</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C709" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>TENSÃO BAIXA</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C710" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>VAZAMENTO DE LUZ</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C711" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>RUÍDO NO ÁUDIO DO MIC/FONE/AUX</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C712" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>CONTROLE COM POUCA SENSIBILIDADE</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C713" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>ABERTURA/GAP</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C714" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>NÃO GRAVA/ATUALIZA</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C715" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>TERRA ABERTO</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C716" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>COATING/SELADOR</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C717" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>ALETA NÃO ABRE/FECHA</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C718" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>EXCESSO DE DÍGITOS</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C719" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>O-CELL COM PELÍCULA</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C720" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>LINHA VERTICAL</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C721" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>POTÊNCIA MÁXIMA</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C722" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>LED NÃO APAGA</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C723" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>INTERFERÊNCIA NA IMAGEM</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C724" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>SEM VÍDEO NO HDMI</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C725" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>LED/DISPLAY PISCANDO</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C726" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>SOFTWARE DESATUALIZADO</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C727" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>VOLUME MÁXIMO NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C728" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>LED COM COR DIFERENTE</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C729" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>PONTO APAGADO</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C730" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>CALÇO/QUADRO APARECENDO</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C731" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>APARELHO NÃO LÊ PEN DRIVE</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C732" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>FALSA FALHA</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C733" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>HI-POT/RIGIDEZ/WI</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C734" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>LED COM LUZ INVERTIDA</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C735" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>EQUIPAMENTO DE TESTE</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C736" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>LINHA HORIZONTAL</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C737" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>RUÍDO NO VENTILADOR</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C738" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>VENTILADOR NÃO GIRA</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C739" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>TECLA DESLOCADA/DANIFICADA</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C740" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>MAL MONTADO</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C741" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>EMPENADO/AMASSADO</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C742" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>TESCON MATERIAL</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C743" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO MIC/FONE/AUX</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C744" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>LIGA/DESLIGA AUTOMATICAMENTE</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C745" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>FALHA VISUAL/MONTAGEM</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C746" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>TESCON FALHA DE PROCESSO</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C747" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>LÂMPADA FRACA/FORTE</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C748" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>CENTELHANDO/RUÍDO</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C749" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>SEM VÍDEO NO RF/ANTENA</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C750" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>LED NÃO ACENDE</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C751" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>FLASH LIGHT NÃO LIGA</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C752" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>APARELHO NÃO DESLIGA</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C753" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>FUNÇÃO INVERTIDA</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C754" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>ÁUDIO OSCILANDO</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C755" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>LÂMPADA NÃO ACENDE</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C756" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>PLACA EM CURTO</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C757" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>CONTROLE NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C758" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>SEM TENSÃO</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C759" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>RISCADO</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C760" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO CANAL DO AF</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C761" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO ALTO-FALANTE</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C762" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>PRATO NÃO GIRA</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C763" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>APARELHO NÃO CARREGA</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C764" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>SEM IMAGEM/SEM BRILHO</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C765" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>MANCHA ESCURA NA TELA</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C766" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>CONTAMINAÇÃO</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C767" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>TECLA DURA</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C768" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>QUEBRADO/DANIFICADO/BATIDO</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C769" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>NÃO COMUNICA</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C770" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>LÂMPADA NÃO APAGA</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C771" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>APARELHO NÃO LIGA</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C772" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>VIBRAÇÃO NO ÁUDIO</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C773" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO CANAL ESQUERDO/FONE</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C774" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>MANCHA</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="C775" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>RUÍDO NO ÁUDIO</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C776" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>VOLUME MÍNIMO NÃO ATUA</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C777" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO CANAL DIREITO/FONE</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C778" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>SEM SINAL DE WI-FI</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C779" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>ESPANADO</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C780" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>TECLAS NÃO ATUAM</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C781" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>VAZAMENTO DE GÁS</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C782" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>VAZAMENTO DE AR</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C783" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>FALTANDO</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>ARCON</t>
+        </is>
+      </c>
+      <c r="C784" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>FORA DO ESPECIFICADO</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C785" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO GERAL</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C786" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>SEM ÁUDIO NO TWEETER</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C787" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>BLUETOOTH NÃO FUNCIONA</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C788" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>NÃO AQUECE</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C789" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>ÁUDIO BAIXO</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C790" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>COM REBARBA</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C791" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>DESLOCADO</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>MWO</t>
+        </is>
+      </c>
+      <c r="C792" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>FALTANDO DÍGITO NO DISPLAY</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C793" s="2" t="n">
+        <v>45968.52253472222</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>